<commit_message>
Update to assignment #1
</commit_message>
<xml_diff>
--- a/StatsAssignment#1/StartUps.xlsx
+++ b/StatsAssignment#1/StartUps.xlsx
@@ -5,17 +5,29 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Trevorcardoza/Documents/GitHub/Statistics/StatsAssignment#1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Trevorcardoza/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497B6A15-72DE-BA41-A401-311C39C16D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F919D095-C202-1348-AAC1-B3005402E08B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$20:$A$26</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$20:$B$26</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$20:$A$26</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$20:$B$26</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$20:$A$26</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$20:$B$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="35" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,18 +42,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>Amount Raised (in Millions)</t>
   </si>
   <si>
-    <t>Relative</t>
+    <t>Row Labels</t>
   </si>
   <si>
-    <t>Percent</t>
+    <t>Grand Total</t>
   </si>
   <si>
-    <t>class dif</t>
+    <t>Count of Amount Raised (in Millions)</t>
+  </si>
+  <si>
+    <t>15-44</t>
+  </si>
+  <si>
+    <t>45-74</t>
+  </si>
+  <si>
+    <t>75-104</t>
+  </si>
+  <si>
+    <t>105-134</t>
+  </si>
+  <si>
+    <t>135-164</t>
+  </si>
+  <si>
+    <t>165-194</t>
+  </si>
+  <si>
+    <t>255-284</t>
+  </si>
+  <si>
+    <t>Rel F</t>
+  </si>
+  <si>
+    <t>Percent F</t>
   </si>
 </sst>
 </file>
@@ -52,7 +91,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,12 +119,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,11 +141,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -129,6 +169,1195 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$20:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15-44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45-74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75-104</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105-134</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135-164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165-194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>255-284</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E80-BD41-984F-B1687D061D49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="359193904"/>
+        <c:axId val="359195536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="359193904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359195536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359195536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359193904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59EF6C84-D7E0-484F-9760-1791452C4334}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Cardoza" refreshedDate="43895.892194675929" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50" xr:uid="{AA3111FE-3AE2-D145-8298-75C22DC9ADCB}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:A51" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Amount Raised (in Millions)" numFmtId="5">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="18" maxValue="272" count="42">
+        <n v="81"/>
+        <n v="80"/>
+        <n v="69"/>
+        <n v="73"/>
+        <n v="192"/>
+        <n v="91"/>
+        <n v="47"/>
+        <n v="154"/>
+        <n v="48"/>
+        <n v="54"/>
+        <n v="61"/>
+        <n v="51"/>
+        <n v="119"/>
+        <n v="50"/>
+        <n v="18"/>
+        <n v="272"/>
+        <n v="24"/>
+        <n v="72"/>
+        <n v="118"/>
+        <n v="112"/>
+        <n v="103"/>
+        <n v="130"/>
+        <n v="110"/>
+        <n v="58"/>
+        <n v="57"/>
+        <n v="38"/>
+        <n v="40"/>
+        <n v="129"/>
+        <n v="166"/>
+        <n v="77"/>
+        <n v="60"/>
+        <n v="21"/>
+        <n v="49"/>
+        <n v="78"/>
+        <n v="131"/>
+        <n v="156"/>
+        <n v="168"/>
+        <n v="20"/>
+        <n v="63"/>
+        <n v="52"/>
+        <n v="55"/>
+        <n v="31"/>
+      </sharedItems>
+      <fieldGroup base="0">
+        <rangePr autoStart="0" autoEnd="0" startNum="15" endNum="284" groupInterval="30"/>
+        <groupItems count="11">
+          <s v="&lt;15"/>
+          <s v="15-44"/>
+          <s v="45-74"/>
+          <s v="75-104"/>
+          <s v="105-134"/>
+          <s v="135-164"/>
+          <s v="165-194"/>
+          <s v="195-224"/>
+          <s v="225-254"/>
+          <s v="255-284"/>
+          <s v="&gt;285"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="50">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="39"/>
+  </r>
+  <r>
+    <x v="40"/>
+  </r>
+  <r>
+    <x v="41"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{931A2A82-6C51-D440-8A45-C80BAD9B2C12}" name="PivotTable9" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" numFmtId="5" showAll="0">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Amount Raised (in Millions)" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,11 +1680,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A817163-0B39-6240-B9B7-757E9E6755C9}">
+  <dimension ref="A3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="Q28" sqref="Q28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",15)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.16</v>
+      </c>
+      <c r="D4" s="7">
+        <f>C4</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",45)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ref="D5:D11" si="0">C5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",75)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.18</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",105)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",135)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.04</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",165)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3,"Amount Raised (in Millions)",255)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <f>GETPIVOTDATA("Amount Raised (in Millions)",$A$3)/GETPIVOTDATA("Amount Raised (in Millions)",$A$3)</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,150 +1927,82 @@
     <col min="2" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>81</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>8</v>
-      </c>
-      <c r="O2" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>80</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=PRODUCT($O2,E2)"),-COUNTIF($A2:$A51,SUM(PRODUCT($O2,E2),"&lt;=-15")))</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=73"),-COUNTIF($A2:$A51,45))</f>
-        <v>23</v>
-      </c>
-      <c r="G3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-      <c r="H3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-      <c r="I3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-      <c r="J3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-      <c r="K3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-      <c r="L3" s="1">
-        <f>SUM(COUNTIF($A2:$A51,"&gt;=44"),-COUNTIF($A2:$A51,15))</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>69</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>18</v>
       </c>
@@ -788,7 +2183,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>